<commit_message>
updated with new Microcredentials
</commit_message>
<xml_diff>
--- a/UC_all.xlsx
+++ b/UC_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3059"/>
+  <dimension ref="A1:H3064"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -79789,7 +79789,7 @@
       </c>
       <c r="B2922" t="inlineStr">
         <is>
-          <t>PROGRAMAÇÃO CAM- ESTRATÉGIAS DE MAQUINAÇÃO A 2,3E5EIXOS</t>
+          <t>PROGRAMAÇÃO CAM - ESTRATÉGIAS DE MAQUINAÇÃO A 2, 3 E 5 EIXOS</t>
         </is>
       </c>
       <c r="C2922" t="inlineStr">
@@ -79802,7 +79802,7 @@
       <c r="F2922" t="inlineStr"/>
       <c r="G2922" t="inlineStr">
         <is>
-          <t>6013_Programação CAM- Estratégias de Maquinação a 2,3e5Eixos</t>
+          <t>6013_Programação CAM - Estratégias de Maquinação a 2, 3 e 5 Eixos</t>
         </is>
       </c>
       <c r="H2922" t="inlineStr"/>
@@ -79837,7 +79837,7 @@
       </c>
       <c r="B2924" t="inlineStr">
         <is>
-          <t>VISÃOARTIFICIAL</t>
+          <t>VISÃO ARTIFICIAL</t>
         </is>
       </c>
       <c r="C2924" t="inlineStr">
@@ -79850,7 +79850,7 @@
       <c r="F2924" t="inlineStr"/>
       <c r="G2924" t="inlineStr">
         <is>
-          <t>6015_VisãoArtificial</t>
+          <t>6015_Visão Artificial</t>
         </is>
       </c>
       <c r="H2924" t="inlineStr"/>
@@ -82369,16 +82369,16 @@
     </row>
     <row r="3025">
       <c r="A3025" t="n">
-        <v>65157</v>
+        <v>65117</v>
       </c>
       <c r="B3025" t="inlineStr">
         <is>
-          <t xml:space="preserve">COMPORTAMENTO E POSES DE VERTEBRADOS </t>
+          <t>DESMATERIALIZAÇÃO NA PRÁTICA DA CONTABILIDADE</t>
         </is>
       </c>
       <c r="C3025" t="inlineStr">
         <is>
-          <t>DBIO</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3025" t="inlineStr"/>
@@ -82386,23 +82386,23 @@
       <c r="F3025" t="inlineStr"/>
       <c r="G3025" t="inlineStr">
         <is>
-          <t xml:space="preserve">6184_Comportamento e Poses de Vertebrados </t>
+          <t>6165_Desmaterialização na Prática da Contabilidade</t>
         </is>
       </c>
       <c r="H3025" t="inlineStr"/>
     </row>
     <row r="3026">
       <c r="A3026" t="n">
-        <v>65117</v>
+        <v>42280</v>
       </c>
       <c r="B3026" t="inlineStr">
         <is>
-          <t>DESMATERIALIZAÇÃO NA PRÁTICA DA CONTABILIDADE</t>
+          <t>FUNDAMENTOS DE CIÊNCIA DE DADOS</t>
         </is>
       </c>
       <c r="C3026" t="inlineStr">
         <is>
-          <t>ISCA</t>
+          <t>DETI</t>
         </is>
       </c>
       <c r="D3026" t="inlineStr"/>
@@ -82410,18 +82410,22 @@
       <c r="F3026" t="inlineStr"/>
       <c r="G3026" t="inlineStr">
         <is>
-          <t>6165_Desmaterialização na Prática da Contabilidade</t>
-        </is>
-      </c>
-      <c r="H3026" t="inlineStr"/>
+          <t>6166_Fundamentos de Ciência de Dados</t>
+        </is>
+      </c>
+      <c r="H3026" t="inlineStr">
+        <is>
+          <t>https://www.ua.pt/en/uc/15542</t>
+        </is>
+      </c>
     </row>
     <row r="3027">
       <c r="A3027" t="n">
-        <v>42280</v>
+        <v>41010</v>
       </c>
       <c r="B3027" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DE CIÊNCIA DE DADOS</t>
+          <t>FUNDAMENTOS DE APRENDIZAGEM AUTOMÁTICA</t>
         </is>
       </c>
       <c r="C3027" t="inlineStr">
@@ -82434,27 +82438,27 @@
       <c r="F3027" t="inlineStr"/>
       <c r="G3027" t="inlineStr">
         <is>
-          <t>6166_Fundamentos de Ciência de Dados</t>
+          <t>6167_Fundamentos de Aprendizagem Automática</t>
         </is>
       </c>
       <c r="H3027" t="inlineStr">
         <is>
-          <t>https://www.ua.pt/en/uc/15542</t>
+          <t>https://www.ua.pt/en/uc/15262</t>
         </is>
       </c>
     </row>
     <row r="3028">
       <c r="A3028" t="n">
-        <v>41010</v>
+        <v>65141</v>
       </c>
       <c r="B3028" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DE APRENDIZAGEM AUTOMÁTICA</t>
+          <t>DIVERSIDADE E ECOLOGIA VEGETAL EM SISTEMAS FLORESTAIS</t>
         </is>
       </c>
       <c r="C3028" t="inlineStr">
         <is>
-          <t>DETI</t>
+          <t>DBIO</t>
         </is>
       </c>
       <c r="D3028" t="inlineStr"/>
@@ -82462,22 +82466,18 @@
       <c r="F3028" t="inlineStr"/>
       <c r="G3028" t="inlineStr">
         <is>
-          <t>6167_Fundamentos de Aprendizagem Automática</t>
-        </is>
-      </c>
-      <c r="H3028" t="inlineStr">
-        <is>
-          <t>https://www.ua.pt/en/uc/15262</t>
-        </is>
-      </c>
+          <t>6169_Diversidade e Ecologia Vegetal em Sistemas Florestais</t>
+        </is>
+      </c>
+      <c r="H3028" t="inlineStr"/>
     </row>
     <row r="3029">
       <c r="A3029" t="n">
-        <v>65141</v>
+        <v>65142</v>
       </c>
       <c r="B3029" t="inlineStr">
         <is>
-          <t>DIVERSIDADE E ECOLOGIA VEGETAL EM SISTEMAS FLORESTAIS</t>
+          <t>DIVERSIDADE E ECOLOGIA ANIMAL EM SISTEMAS FLORESTAIS - VERTEBRADOS</t>
         </is>
       </c>
       <c r="C3029" t="inlineStr">
@@ -82490,18 +82490,18 @@
       <c r="F3029" t="inlineStr"/>
       <c r="G3029" t="inlineStr">
         <is>
-          <t>6169_Diversidade e Ecologia Vegetal em Sistemas Florestais</t>
+          <t>6170_Diversidade e Ecologia Animal em Sistemas Florestais - Vertebrados</t>
         </is>
       </c>
       <c r="H3029" t="inlineStr"/>
     </row>
     <row r="3030">
       <c r="A3030" t="n">
-        <v>65142</v>
+        <v>65143</v>
       </c>
       <c r="B3030" t="inlineStr">
         <is>
-          <t>DIVERSIDADE E ECOLOGIA ANIMAL EM SISTEMAS FLORESTAIS - VERTEBRADOS</t>
+          <t>DIVERSIDADE E ECOLOGIA ANIMAL EM SISTEMAS FLORESTAIS - INSETOS E OUTROS INVERTEBRADOS</t>
         </is>
       </c>
       <c r="C3030" t="inlineStr">
@@ -82514,18 +82514,18 @@
       <c r="F3030" t="inlineStr"/>
       <c r="G3030" t="inlineStr">
         <is>
-          <t>6170_Diversidade e Ecologia Animal em Sistemas Florestais - Vertebrados</t>
+          <t>6171_Diversidade e Ecologia Animal em Sistemas Florestais - Insetos E Outros Invertebrados</t>
         </is>
       </c>
       <c r="H3030" t="inlineStr"/>
     </row>
     <row r="3031">
       <c r="A3031" t="n">
-        <v>65143</v>
+        <v>65144</v>
       </c>
       <c r="B3031" t="inlineStr">
         <is>
-          <t>DIVERSIDADE E ECOLOGIA ANIMAL EM SISTEMAS FLORESTAIS - INSETOS E OUTROS INVERTEBRADOS</t>
+          <t>BIODIVERSIDADE E SERVIÇOS DE ECOSSISTEMAS EM SISTEMAS FLORESTAIS</t>
         </is>
       </c>
       <c r="C3031" t="inlineStr">
@@ -82538,18 +82538,18 @@
       <c r="F3031" t="inlineStr"/>
       <c r="G3031" t="inlineStr">
         <is>
-          <t>6171_Diversidade e Ecologia Animal em Sistemas Florestais - Insetos E Outros Invertebrados</t>
+          <t>6172_Biodiversidade e Serviços de Ecossistemas em Sistemas Florestais</t>
         </is>
       </c>
       <c r="H3031" t="inlineStr"/>
     </row>
     <row r="3032">
       <c r="A3032" t="n">
-        <v>65144</v>
+        <v>65145</v>
       </c>
       <c r="B3032" t="inlineStr">
         <is>
-          <t>BIODIVERSIDADE E SERVIÇOS EE ECOSSISTEMAS EM SISTEMAS FLORESTAIS</t>
+          <t>UTILIZAÇÃO DE SUBSTÂNCIAS BIOATIVAS EM CONTEXTO DE PRODUÇÃO ANIMAL</t>
         </is>
       </c>
       <c r="C3032" t="inlineStr">
@@ -82562,23 +82562,23 @@
       <c r="F3032" t="inlineStr"/>
       <c r="G3032" t="inlineStr">
         <is>
-          <t>6172_Biodiversidade e Serviços ee Ecossistemas em Sistemas Florestais</t>
+          <t>6173_Utilização de Substâncias Bioativas em Contexto de Produção Animal</t>
         </is>
       </c>
       <c r="H3032" t="inlineStr"/>
     </row>
     <row r="3033">
       <c r="A3033" t="n">
-        <v>65145</v>
+        <v>65146</v>
       </c>
       <c r="B3033" t="inlineStr">
         <is>
-          <t>UTILIZAÇÃO DE SUBSTÂNCIAS BIOATIVAS EM CONTEXTO DE PRODUÇÃO ANIMAL</t>
+          <t>INTRODUÇÃO À VISÃO COMPUTACIONAL COM PYTORCH</t>
         </is>
       </c>
       <c r="C3033" t="inlineStr">
         <is>
-          <t>DBIO</t>
+          <t>DMAT</t>
         </is>
       </c>
       <c r="D3033" t="inlineStr"/>
@@ -82586,18 +82586,18 @@
       <c r="F3033" t="inlineStr"/>
       <c r="G3033" t="inlineStr">
         <is>
-          <t>6173_Utilização de Substâncias Bioativas em Contexto de Produção Animal</t>
+          <t>6174_Introdução à visão computacional com PyTorch</t>
         </is>
       </c>
       <c r="H3033" t="inlineStr"/>
     </row>
     <row r="3034">
       <c r="A3034" t="n">
-        <v>65146</v>
+        <v>65147</v>
       </c>
       <c r="B3034" t="inlineStr">
         <is>
-          <t>INTRODUÇÃO À VISÃO COMPUTACIONAL COM PYTORCH</t>
+          <t>ALGORITMOS INTELIGENTES PARA DADOS INDUSTRIAIS</t>
         </is>
       </c>
       <c r="C3034" t="inlineStr">
@@ -82610,18 +82610,18 @@
       <c r="F3034" t="inlineStr"/>
       <c r="G3034" t="inlineStr">
         <is>
-          <t>6174_Introdução à visão computacional com PyTorch</t>
+          <t>6175_Algoritmos Inteligentes para Dados Industriais</t>
         </is>
       </c>
       <c r="H3034" t="inlineStr"/>
     </row>
     <row r="3035">
       <c r="A3035" t="n">
-        <v>65147</v>
+        <v>65148</v>
       </c>
       <c r="B3035" t="inlineStr">
         <is>
-          <t>ALGORITMOS INTELIGENTES PARA DADOS INDUSTRIAIS</t>
+          <t>ANÁLISE, OTIMIZAÇÃO E AVALIAÇÃO COMPARATIVA DE PROCESSOS INDUSTRIAIS E LOGÍSTICOS</t>
         </is>
       </c>
       <c r="C3035" t="inlineStr">
@@ -82634,23 +82634,23 @@
       <c r="F3035" t="inlineStr"/>
       <c r="G3035" t="inlineStr">
         <is>
-          <t>6175_Algoritmos Inteligentes para Dados Industriais</t>
+          <t>6176_Análise, Otimização e Avaliação Comparativa de Processos Industriais e Logísticos</t>
         </is>
       </c>
       <c r="H3035" t="inlineStr"/>
     </row>
     <row r="3036">
       <c r="A3036" t="n">
-        <v>65148</v>
+        <v>65150</v>
       </c>
       <c r="B3036" t="inlineStr">
         <is>
-          <t>ANÁLISE, OTIMIZAÇÃO E AVALIAÇÃO COMPARATIVA DE PROCESSOS INDUSTRIAIS E LOGÍSTICOS</t>
+          <t>BIOMETRIA: A PRÓXIMA GERAÇÃO DE SEGURANÇA</t>
         </is>
       </c>
       <c r="C3036" t="inlineStr">
         <is>
-          <t>DMAT</t>
+          <t>DETI</t>
         </is>
       </c>
       <c r="D3036" t="inlineStr"/>
@@ -82658,18 +82658,18 @@
       <c r="F3036" t="inlineStr"/>
       <c r="G3036" t="inlineStr">
         <is>
-          <t>6176_Análise, Otimização e Avaliação Comparativa de Processos Industriais e Logísticos</t>
+          <t>6177_Biometria: a próxima geração de segurança</t>
         </is>
       </c>
       <c r="H3036" t="inlineStr"/>
     </row>
     <row r="3037">
       <c r="A3037" t="n">
-        <v>65150</v>
+        <v>65151</v>
       </c>
       <c r="B3037" t="inlineStr">
         <is>
-          <t>BIOMETRIA: A PRÓXIMA GERAÇÃO DE SEGURANÇA</t>
+          <t>PROGRAMAÇÃO POR OBJETOS (POO) EM C++</t>
         </is>
       </c>
       <c r="C3037" t="inlineStr">
@@ -82682,18 +82682,18 @@
       <c r="F3037" t="inlineStr"/>
       <c r="G3037" t="inlineStr">
         <is>
-          <t>6177_Biometria: a próxima geração de segurança</t>
+          <t>6179_Programação por objetos (POO) em C++</t>
         </is>
       </c>
       <c r="H3037" t="inlineStr"/>
     </row>
     <row r="3038">
       <c r="A3038" t="n">
-        <v>65151</v>
+        <v>65152</v>
       </c>
       <c r="B3038" t="inlineStr">
         <is>
-          <t>PROGRAMAÇÃO POR OBJETOS (POO) EM C++</t>
+          <t>PROGRAMAÇÃO EM PYTHON PARA ANÁLISE DE DADOS</t>
         </is>
       </c>
       <c r="C3038" t="inlineStr">
@@ -82706,18 +82706,18 @@
       <c r="F3038" t="inlineStr"/>
       <c r="G3038" t="inlineStr">
         <is>
-          <t>6179_Programação por objetos (POO) em C++</t>
+          <t>6180_Programação em Python para análise de dados</t>
         </is>
       </c>
       <c r="H3038" t="inlineStr"/>
     </row>
     <row r="3039">
       <c r="A3039" t="n">
-        <v>65152</v>
+        <v>65153</v>
       </c>
       <c r="B3039" t="inlineStr">
         <is>
-          <t>PROGRAMAÇÃO EM PYTHON PARA ANÁLISE DE DADOS</t>
+          <t>CARACTERIZAÇÃO DE DISPOSITIVOS DE MICROONDAS E ANTENAS</t>
         </is>
       </c>
       <c r="C3039" t="inlineStr">
@@ -82730,18 +82730,18 @@
       <c r="F3039" t="inlineStr"/>
       <c r="G3039" t="inlineStr">
         <is>
-          <t>6180_Programação em Python para análise de dados</t>
+          <t>6181_Caracterização de Dispositivos de Microondas e Antenas</t>
         </is>
       </c>
       <c r="H3039" t="inlineStr"/>
     </row>
     <row r="3040">
       <c r="A3040" t="n">
-        <v>65153</v>
+        <v>65154</v>
       </c>
       <c r="B3040" t="inlineStr">
         <is>
-          <t>CARACTERIZAÇÃO DE DISPOSITIVOS DE MICROONDAS E ANTENAS</t>
+          <t>CIRCUITOS DC E AC</t>
         </is>
       </c>
       <c r="C3040" t="inlineStr">
@@ -82754,18 +82754,18 @@
       <c r="F3040" t="inlineStr"/>
       <c r="G3040" t="inlineStr">
         <is>
-          <t>6181_Caracterização de Dispositivos de Microondas e Antenas</t>
+          <t>6182_Circuitos DC e AC</t>
         </is>
       </c>
       <c r="H3040" t="inlineStr"/>
     </row>
     <row r="3041">
       <c r="A3041" t="n">
-        <v>65154</v>
+        <v>65155</v>
       </c>
       <c r="B3041" t="inlineStr">
         <is>
-          <t>CIRCUITOS DC E AC</t>
+          <t>INSTRUMENTAÇÃO E MEDIDAS EM MICROONDAS</t>
         </is>
       </c>
       <c r="C3041" t="inlineStr">
@@ -82778,23 +82778,23 @@
       <c r="F3041" t="inlineStr"/>
       <c r="G3041" t="inlineStr">
         <is>
-          <t>6182_Circuitos DC e AC</t>
+          <t>6183_Instrumentação e Medidas em Microondas</t>
         </is>
       </c>
       <c r="H3041" t="inlineStr"/>
     </row>
     <row r="3042">
       <c r="A3042" t="n">
-        <v>65155</v>
+        <v>65157</v>
       </c>
       <c r="B3042" t="inlineStr">
         <is>
-          <t>INSTRUMENTAÇÃO E MEDIDAS EM MICROONDAS</t>
+          <t xml:space="preserve">COMPORTAMENTO E POSES DE VERTEBRADOS </t>
         </is>
       </c>
       <c r="C3042" t="inlineStr">
         <is>
-          <t>DETI</t>
+          <t>DBIO</t>
         </is>
       </c>
       <c r="D3042" t="inlineStr"/>
@@ -82802,7 +82802,7 @@
       <c r="F3042" t="inlineStr"/>
       <c r="G3042" t="inlineStr">
         <is>
-          <t>6183_Instrumentação e Medidas em Microondas</t>
+          <t xml:space="preserve">6184_Comportamento e Poses de Vertebrados </t>
         </is>
       </c>
       <c r="H3042" t="inlineStr"/>
@@ -82905,16 +82905,16 @@
     </row>
     <row r="3047">
       <c r="A3047" t="n">
-        <v>65030</v>
+        <v>65171</v>
       </c>
       <c r="B3047" t="inlineStr">
         <is>
-          <t>DESIGN DE INTERAÇÃO PARA A EXPERIÊNCIA</t>
+          <t>ANÁLISE FINANCEIRA PARA NÃO FINANCEIROS</t>
         </is>
       </c>
       <c r="C3047" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3047" t="inlineStr"/>
@@ -82922,23 +82922,23 @@
       <c r="F3047" t="inlineStr"/>
       <c r="G3047" t="inlineStr">
         <is>
-          <t>6530_Design de Interação para a eXperiência</t>
+          <t>6189_Análise Financeira para Não Financeiros</t>
         </is>
       </c>
       <c r="H3047" t="inlineStr"/>
     </row>
     <row r="3048">
       <c r="A3048" t="n">
-        <v>65082</v>
+        <v>65175</v>
       </c>
       <c r="B3048" t="inlineStr">
         <is>
-          <t>TECNOLOGIASINOVADORASDECONSERVAÇÃOEMODIFICAÇÃODEALIMENTOS</t>
+          <t>CONTABILIDADE E FISCALIDADE PARA NÃO FINANCEIROS</t>
         </is>
       </c>
       <c r="C3048" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3048" t="inlineStr"/>
@@ -82946,23 +82946,23 @@
       <c r="F3048" t="inlineStr"/>
       <c r="G3048" t="inlineStr">
         <is>
-          <t>6531_TecnologiasInovadorasdeConservaçãoeModificaçãodeAlimentos</t>
+          <t>6190_Contabilidade e Fiscalidade para Não Financeiros</t>
         </is>
       </c>
       <c r="H3048" t="inlineStr"/>
     </row>
     <row r="3049">
       <c r="A3049" t="n">
-        <v>65084</v>
+        <v>65172</v>
       </c>
       <c r="B3049" t="inlineStr">
         <is>
-          <t>PERCEÇÃO MULTISSENSORIAL DE ALIMENTOS</t>
+          <t>BUSINESS INTELLIGENCE E ANÁLISE DE DADOS COM POWER BI</t>
         </is>
       </c>
       <c r="C3049" t="inlineStr">
         <is>
-          <t>DEP</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3049" t="inlineStr"/>
@@ -82970,23 +82970,23 @@
       <c r="F3049" t="inlineStr"/>
       <c r="G3049" t="inlineStr">
         <is>
-          <t>6532_Perceção Multissensorial de Alimentos</t>
+          <t>6191_Business Intelligence e Análise de Dados com Power Bi</t>
         </is>
       </c>
       <c r="H3049" t="inlineStr"/>
     </row>
     <row r="3050">
       <c r="A3050" t="n">
-        <v>65091</v>
+        <v>65174</v>
       </c>
       <c r="B3050" t="inlineStr">
         <is>
-          <t>CRIAÇÃO DE CONTEÚDOS AUDIOVISUAIS PARA NOVOS MÉDIA</t>
+          <t>DIREITO APLICADO AO MARKETING DIGITAL</t>
         </is>
       </c>
       <c r="C3050" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3050" t="inlineStr"/>
@@ -82994,23 +82994,23 @@
       <c r="F3050" t="inlineStr"/>
       <c r="G3050" t="inlineStr">
         <is>
-          <t>6533_Criação de conteúdos audiovisuais para Novos Média</t>
+          <t>6192_Direito Aplicado ao Marketing Digital</t>
         </is>
       </c>
       <c r="H3050" t="inlineStr"/>
     </row>
     <row r="3051">
       <c r="A3051" t="n">
-        <v>65092</v>
+        <v>65170</v>
       </c>
       <c r="B3051" t="inlineStr">
         <is>
-          <t>INTERFACES DE REALIDADE VIRTUAL</t>
+          <t>INTELIGÊNCIA ARTIFICIAL GENERATIVA EM MARKETING DIGITAL</t>
         </is>
       </c>
       <c r="C3051" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>ISCA</t>
         </is>
       </c>
       <c r="D3051" t="inlineStr"/>
@@ -83018,18 +83018,18 @@
       <c r="F3051" t="inlineStr"/>
       <c r="G3051" t="inlineStr">
         <is>
-          <t>6534_Interfaces de Realidade Virtual</t>
+          <t>6193_Inteligência Artificial Generativa em Marketing Digital</t>
         </is>
       </c>
       <c r="H3051" t="inlineStr"/>
     </row>
     <row r="3052">
       <c r="A3052" t="n">
-        <v>65093</v>
+        <v>65030</v>
       </c>
       <c r="B3052" t="inlineStr">
         <is>
-          <t>INTERFACES WEB COM JAVASCRIPT</t>
+          <t>DESIGN DE INTERAÇÃO PARA A EXPERIÊNCIA</t>
         </is>
       </c>
       <c r="C3052" t="inlineStr">
@@ -83042,23 +83042,23 @@
       <c r="F3052" t="inlineStr"/>
       <c r="G3052" t="inlineStr">
         <is>
-          <t>6535_Interfaces Web com JavaScript</t>
+          <t>6530_Design de Interação para a eXperiência</t>
         </is>
       </c>
       <c r="H3052" t="inlineStr"/>
     </row>
     <row r="3053">
       <c r="A3053" t="n">
-        <v>65094</v>
+        <v>65082</v>
       </c>
       <c r="B3053" t="inlineStr">
         <is>
-          <t>JOGOS SÉRIOS</t>
+          <t>TECNOLOGIASINOVADORASDECONSERVAÇÃOEMODIFICAÇÃODEALIMENTOS</t>
         </is>
       </c>
       <c r="C3053" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="D3053" t="inlineStr"/>
@@ -83066,23 +83066,23 @@
       <c r="F3053" t="inlineStr"/>
       <c r="G3053" t="inlineStr">
         <is>
-          <t>6536_Jogos Sérios</t>
+          <t>6531_TecnologiasInovadorasdeConservaçãoeModificaçãodeAlimentos</t>
         </is>
       </c>
       <c r="H3053" t="inlineStr"/>
     </row>
     <row r="3054">
       <c r="A3054" t="n">
-        <v>65095</v>
+        <v>65084</v>
       </c>
       <c r="B3054" t="inlineStr">
         <is>
-          <t>PRODUÇÃO AUDIOVISUAL DIGITAL PARA FICÇÃO/NÃOFICÇÃO</t>
+          <t>PERCEÇÃO MULTISSENSORIAL DE ALIMENTOS</t>
         </is>
       </c>
       <c r="C3054" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>DEP</t>
         </is>
       </c>
       <c r="D3054" t="inlineStr"/>
@@ -83090,18 +83090,18 @@
       <c r="F3054" t="inlineStr"/>
       <c r="G3054" t="inlineStr">
         <is>
-          <t>6537_Produção Audiovisual Digital para Ficção/NãoFicção</t>
+          <t>6532_Perceção Multissensorial de Alimentos</t>
         </is>
       </c>
       <c r="H3054" t="inlineStr"/>
     </row>
     <row r="3055">
       <c r="A3055" t="n">
-        <v>65096</v>
+        <v>65091</v>
       </c>
       <c r="B3055" t="inlineStr">
         <is>
-          <t>STORYTELLING DIGITAL</t>
+          <t>CRIAÇÃO DE CONTEÚDOS AUDIOVISUAIS PARA NOVOS MÉDIA</t>
         </is>
       </c>
       <c r="C3055" t="inlineStr">
@@ -83114,18 +83114,18 @@
       <c r="F3055" t="inlineStr"/>
       <c r="G3055" t="inlineStr">
         <is>
-          <t>6538_Storytelling Digital</t>
+          <t>6533_Criação de conteúdos audiovisuais para Novos Média</t>
         </is>
       </c>
       <c r="H3055" t="inlineStr"/>
     </row>
     <row r="3056">
       <c r="A3056" t="n">
-        <v>65097</v>
+        <v>65092</v>
       </c>
       <c r="B3056" t="inlineStr">
         <is>
-          <t>TÉCNICAS CONTEMPORÂNEAS DE COMPOSIÇÃO E ARRANJO EM JAZZ</t>
+          <t>INTERFACES DE REALIDADE VIRTUAL</t>
         </is>
       </c>
       <c r="C3056" t="inlineStr">
@@ -83138,23 +83138,23 @@
       <c r="F3056" t="inlineStr"/>
       <c r="G3056" t="inlineStr">
         <is>
-          <t>6539_Técnicas Contemporâneas de Composição e Arranjo em Jazz</t>
+          <t>6534_Interfaces de Realidade Virtual</t>
         </is>
       </c>
       <c r="H3056" t="inlineStr"/>
     </row>
     <row r="3057">
       <c r="A3057" t="n">
-        <v>65158</v>
+        <v>65093</v>
       </c>
       <c r="B3057" t="inlineStr">
         <is>
-          <t xml:space="preserve">GEOLOGIA DE CAMPO - AMBIENTES SEDIMENTARES </t>
+          <t>INTERFACES WEB COM JAVASCRIPT</t>
         </is>
       </c>
       <c r="C3057" t="inlineStr">
         <is>
-          <t>DGEO</t>
+          <t>DECA</t>
         </is>
       </c>
       <c r="D3057" t="inlineStr"/>
@@ -83162,23 +83162,23 @@
       <c r="F3057" t="inlineStr"/>
       <c r="G3057" t="inlineStr">
         <is>
-          <t xml:space="preserve">6542_Geologia de Campo - Ambientes Sedimentares </t>
+          <t>6535_Interfaces Web com JavaScript</t>
         </is>
       </c>
       <c r="H3057" t="inlineStr"/>
     </row>
     <row r="3058">
       <c r="A3058" t="n">
-        <v>65159</v>
+        <v>65094</v>
       </c>
       <c r="B3058" t="inlineStr">
         <is>
-          <t xml:space="preserve">GEOLOGIA DE CAMPO – ROCHAS METAMÓRFICAS </t>
+          <t>JOGOS SÉRIOS</t>
         </is>
       </c>
       <c r="C3058" t="inlineStr">
         <is>
-          <t>DGEO</t>
+          <t>DECA</t>
         </is>
       </c>
       <c r="D3058" t="inlineStr"/>
@@ -83186,23 +83186,23 @@
       <c r="F3058" t="inlineStr"/>
       <c r="G3058" t="inlineStr">
         <is>
-          <t xml:space="preserve">6543_Geologia de Campo – Rochas Metamórficas </t>
+          <t>6536_Jogos Sérios</t>
         </is>
       </c>
       <c r="H3058" t="inlineStr"/>
     </row>
     <row r="3059">
       <c r="A3059" t="n">
-        <v>65160</v>
+        <v>65095</v>
       </c>
       <c r="B3059" t="inlineStr">
         <is>
-          <t>GEOLOGIA DE CAMPO – ROCHAS ÍGNEAS</t>
+          <t>PRODUÇÃO AUDIOVISUAL DIGITAL PARA FICÇÃO/NÃOFICÇÃO</t>
         </is>
       </c>
       <c r="C3059" t="inlineStr">
         <is>
-          <t>DGEO</t>
+          <t>DECA</t>
         </is>
       </c>
       <c r="D3059" t="inlineStr"/>
@@ -83210,10 +83210,130 @@
       <c r="F3059" t="inlineStr"/>
       <c r="G3059" t="inlineStr">
         <is>
+          <t>6537_Produção Audiovisual Digital para Ficção/NãoFicção</t>
+        </is>
+      </c>
+      <c r="H3059" t="inlineStr"/>
+    </row>
+    <row r="3060">
+      <c r="A3060" t="n">
+        <v>65096</v>
+      </c>
+      <c r="B3060" t="inlineStr">
+        <is>
+          <t>STORYTELLING DIGITAL</t>
+        </is>
+      </c>
+      <c r="C3060" t="inlineStr">
+        <is>
+          <t>DECA</t>
+        </is>
+      </c>
+      <c r="D3060" t="inlineStr"/>
+      <c r="E3060" t="inlineStr"/>
+      <c r="F3060" t="inlineStr"/>
+      <c r="G3060" t="inlineStr">
+        <is>
+          <t>6538_Storytelling Digital</t>
+        </is>
+      </c>
+      <c r="H3060" t="inlineStr"/>
+    </row>
+    <row r="3061">
+      <c r="A3061" t="n">
+        <v>65097</v>
+      </c>
+      <c r="B3061" t="inlineStr">
+        <is>
+          <t>TÉCNICAS CONTEMPORÂNEAS DE COMPOSIÇÃO E ARRANJO EM JAZZ</t>
+        </is>
+      </c>
+      <c r="C3061" t="inlineStr">
+        <is>
+          <t>DECA</t>
+        </is>
+      </c>
+      <c r="D3061" t="inlineStr"/>
+      <c r="E3061" t="inlineStr"/>
+      <c r="F3061" t="inlineStr"/>
+      <c r="G3061" t="inlineStr">
+        <is>
+          <t>6539_Técnicas Contemporâneas de Composição e Arranjo em Jazz</t>
+        </is>
+      </c>
+      <c r="H3061" t="inlineStr"/>
+    </row>
+    <row r="3062">
+      <c r="A3062" t="n">
+        <v>65158</v>
+      </c>
+      <c r="B3062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEOLOGIA DE CAMPO - AMBIENTES SEDIMENTARES </t>
+        </is>
+      </c>
+      <c r="C3062" t="inlineStr">
+        <is>
+          <t>DGEO</t>
+        </is>
+      </c>
+      <c r="D3062" t="inlineStr"/>
+      <c r="E3062" t="inlineStr"/>
+      <c r="F3062" t="inlineStr"/>
+      <c r="G3062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6542_Geologia de Campo - Ambientes Sedimentares </t>
+        </is>
+      </c>
+      <c r="H3062" t="inlineStr"/>
+    </row>
+    <row r="3063">
+      <c r="A3063" t="n">
+        <v>65159</v>
+      </c>
+      <c r="B3063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEOLOGIA DE CAMPO – ROCHAS METAMÓRFICAS </t>
+        </is>
+      </c>
+      <c r="C3063" t="inlineStr">
+        <is>
+          <t>DGEO</t>
+        </is>
+      </c>
+      <c r="D3063" t="inlineStr"/>
+      <c r="E3063" t="inlineStr"/>
+      <c r="F3063" t="inlineStr"/>
+      <c r="G3063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6543_Geologia de Campo – Rochas Metamórficas </t>
+        </is>
+      </c>
+      <c r="H3063" t="inlineStr"/>
+    </row>
+    <row r="3064">
+      <c r="A3064" t="n">
+        <v>65160</v>
+      </c>
+      <c r="B3064" t="inlineStr">
+        <is>
+          <t>GEOLOGIA DE CAMPO – ROCHAS ÍGNEAS</t>
+        </is>
+      </c>
+      <c r="C3064" t="inlineStr">
+        <is>
+          <t>DGEO</t>
+        </is>
+      </c>
+      <c r="D3064" t="inlineStr"/>
+      <c r="E3064" t="inlineStr"/>
+      <c r="F3064" t="inlineStr"/>
+      <c r="G3064" t="inlineStr">
+        <is>
           <t>6544_Geologia de Campo – Rochas Ígneas</t>
         </is>
       </c>
-      <c r="H3059" t="inlineStr"/>
+      <c r="H3064" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
small fix to microcrendtials
</commit_message>
<xml_diff>
--- a/UC_all.xlsx
+++ b/UC_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3064"/>
+  <dimension ref="A1:H3065"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -83025,16 +83025,16 @@
     </row>
     <row r="3052">
       <c r="A3052" t="n">
-        <v>65030</v>
+        <v>65173</v>
       </c>
       <c r="B3052" t="inlineStr">
         <is>
-          <t>DESIGN DE INTERAÇÃO PARA A EXPERIÊNCIA</t>
+          <t>AVALIAÇÃO DA SEGURANÇA SÍSMICA DE EDIFÍCIOS EXISTENTES DE BETÃO ARMADO</t>
         </is>
       </c>
       <c r="C3052" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>DCIVIL</t>
         </is>
       </c>
       <c r="D3052" t="inlineStr"/>
@@ -83042,23 +83042,23 @@
       <c r="F3052" t="inlineStr"/>
       <c r="G3052" t="inlineStr">
         <is>
-          <t>6530_Design de Interação para a eXperiência</t>
+          <t>6194_Avaliação da Segurança Sísmica de Edifícios Existentes de Betão Armado</t>
         </is>
       </c>
       <c r="H3052" t="inlineStr"/>
     </row>
     <row r="3053">
       <c r="A3053" t="n">
-        <v>65082</v>
+        <v>65030</v>
       </c>
       <c r="B3053" t="inlineStr">
         <is>
-          <t>TECNOLOGIASINOVADORASDECONSERVAÇÃOEMODIFICAÇÃODEALIMENTOS</t>
+          <t>DESIGN DE INTERAÇÃO PARA A EXPERIÊNCIA</t>
         </is>
       </c>
       <c r="C3053" t="inlineStr">
         <is>
-          <t>DQ</t>
+          <t>DECA</t>
         </is>
       </c>
       <c r="D3053" t="inlineStr"/>
@@ -83066,23 +83066,23 @@
       <c r="F3053" t="inlineStr"/>
       <c r="G3053" t="inlineStr">
         <is>
-          <t>6531_TecnologiasInovadorasdeConservaçãoeModificaçãodeAlimentos</t>
+          <t>6530_Design de Interação para a eXperiência</t>
         </is>
       </c>
       <c r="H3053" t="inlineStr"/>
     </row>
     <row r="3054">
       <c r="A3054" t="n">
-        <v>65084</v>
+        <v>65082</v>
       </c>
       <c r="B3054" t="inlineStr">
         <is>
-          <t>PERCEÇÃO MULTISSENSORIAL DE ALIMENTOS</t>
+          <t>TECNOLOGIASINOVADORASDECONSERVAÇÃOEMODIFICAÇÃODEALIMENTOS</t>
         </is>
       </c>
       <c r="C3054" t="inlineStr">
         <is>
-          <t>DEP</t>
+          <t>DQ</t>
         </is>
       </c>
       <c r="D3054" t="inlineStr"/>
@@ -83090,23 +83090,23 @@
       <c r="F3054" t="inlineStr"/>
       <c r="G3054" t="inlineStr">
         <is>
-          <t>6532_Perceção Multissensorial de Alimentos</t>
+          <t>6531_TecnologiasInovadorasdeConservaçãoeModificaçãodeAlimentos</t>
         </is>
       </c>
       <c r="H3054" t="inlineStr"/>
     </row>
     <row r="3055">
       <c r="A3055" t="n">
-        <v>65091</v>
+        <v>65084</v>
       </c>
       <c r="B3055" t="inlineStr">
         <is>
-          <t>CRIAÇÃO DE CONTEÚDOS AUDIOVISUAIS PARA NOVOS MÉDIA</t>
+          <t>PERCEÇÃO MULTISSENSORIAL DE ALIMENTOS</t>
         </is>
       </c>
       <c r="C3055" t="inlineStr">
         <is>
-          <t>DECA</t>
+          <t>DEP</t>
         </is>
       </c>
       <c r="D3055" t="inlineStr"/>
@@ -83114,18 +83114,18 @@
       <c r="F3055" t="inlineStr"/>
       <c r="G3055" t="inlineStr">
         <is>
-          <t>6533_Criação de conteúdos audiovisuais para Novos Média</t>
+          <t>6532_Perceção Multissensorial de Alimentos</t>
         </is>
       </c>
       <c r="H3055" t="inlineStr"/>
     </row>
     <row r="3056">
       <c r="A3056" t="n">
-        <v>65092</v>
+        <v>65091</v>
       </c>
       <c r="B3056" t="inlineStr">
         <is>
-          <t>INTERFACES DE REALIDADE VIRTUAL</t>
+          <t>CRIAÇÃO DE CONTEÚDOS AUDIOVISUAIS PARA NOVOS MÉDIA</t>
         </is>
       </c>
       <c r="C3056" t="inlineStr">
@@ -83138,18 +83138,18 @@
       <c r="F3056" t="inlineStr"/>
       <c r="G3056" t="inlineStr">
         <is>
-          <t>6534_Interfaces de Realidade Virtual</t>
+          <t>6533_Criação de conteúdos audiovisuais para Novos Média</t>
         </is>
       </c>
       <c r="H3056" t="inlineStr"/>
     </row>
     <row r="3057">
       <c r="A3057" t="n">
-        <v>65093</v>
+        <v>65092</v>
       </c>
       <c r="B3057" t="inlineStr">
         <is>
-          <t>INTERFACES WEB COM JAVASCRIPT</t>
+          <t>INTERFACES DE REALIDADE VIRTUAL</t>
         </is>
       </c>
       <c r="C3057" t="inlineStr">
@@ -83162,18 +83162,18 @@
       <c r="F3057" t="inlineStr"/>
       <c r="G3057" t="inlineStr">
         <is>
-          <t>6535_Interfaces Web com JavaScript</t>
+          <t>6534_Interfaces de Realidade Virtual</t>
         </is>
       </c>
       <c r="H3057" t="inlineStr"/>
     </row>
     <row r="3058">
       <c r="A3058" t="n">
-        <v>65094</v>
+        <v>65093</v>
       </c>
       <c r="B3058" t="inlineStr">
         <is>
-          <t>JOGOS SÉRIOS</t>
+          <t>INTERFACES WEB COM JAVASCRIPT</t>
         </is>
       </c>
       <c r="C3058" t="inlineStr">
@@ -83186,18 +83186,18 @@
       <c r="F3058" t="inlineStr"/>
       <c r="G3058" t="inlineStr">
         <is>
-          <t>6536_Jogos Sérios</t>
+          <t>6535_Interfaces Web com JavaScript</t>
         </is>
       </c>
       <c r="H3058" t="inlineStr"/>
     </row>
     <row r="3059">
       <c r="A3059" t="n">
-        <v>65095</v>
+        <v>65094</v>
       </c>
       <c r="B3059" t="inlineStr">
         <is>
-          <t>PRODUÇÃO AUDIOVISUAL DIGITAL PARA FICÇÃO/NÃOFICÇÃO</t>
+          <t>JOGOS SÉRIOS</t>
         </is>
       </c>
       <c r="C3059" t="inlineStr">
@@ -83210,18 +83210,18 @@
       <c r="F3059" t="inlineStr"/>
       <c r="G3059" t="inlineStr">
         <is>
-          <t>6537_Produção Audiovisual Digital para Ficção/NãoFicção</t>
+          <t>6536_Jogos Sérios</t>
         </is>
       </c>
       <c r="H3059" t="inlineStr"/>
     </row>
     <row r="3060">
       <c r="A3060" t="n">
-        <v>65096</v>
+        <v>65095</v>
       </c>
       <c r="B3060" t="inlineStr">
         <is>
-          <t>STORYTELLING DIGITAL</t>
+          <t>PRODUÇÃO AUDIOVISUAL DIGITAL PARA FICÇÃO/NÃOFICÇÃO</t>
         </is>
       </c>
       <c r="C3060" t="inlineStr">
@@ -83234,18 +83234,18 @@
       <c r="F3060" t="inlineStr"/>
       <c r="G3060" t="inlineStr">
         <is>
-          <t>6538_Storytelling Digital</t>
+          <t>6537_Produção Audiovisual Digital para Ficção/NãoFicção</t>
         </is>
       </c>
       <c r="H3060" t="inlineStr"/>
     </row>
     <row r="3061">
       <c r="A3061" t="n">
-        <v>65097</v>
+        <v>65096</v>
       </c>
       <c r="B3061" t="inlineStr">
         <is>
-          <t>TÉCNICAS CONTEMPORÂNEAS DE COMPOSIÇÃO E ARRANJO EM JAZZ</t>
+          <t>STORYTELLING DIGITAL</t>
         </is>
       </c>
       <c r="C3061" t="inlineStr">
@@ -83258,23 +83258,23 @@
       <c r="F3061" t="inlineStr"/>
       <c r="G3061" t="inlineStr">
         <is>
-          <t>6539_Técnicas Contemporâneas de Composição e Arranjo em Jazz</t>
+          <t>6538_Storytelling Digital</t>
         </is>
       </c>
       <c r="H3061" t="inlineStr"/>
     </row>
     <row r="3062">
       <c r="A3062" t="n">
-        <v>65158</v>
+        <v>65097</v>
       </c>
       <c r="B3062" t="inlineStr">
         <is>
-          <t xml:space="preserve">GEOLOGIA DE CAMPO - AMBIENTES SEDIMENTARES </t>
+          <t>TÉCNICAS CONTEMPORÂNEAS DE COMPOSIÇÃO E ARRANJO EM JAZZ</t>
         </is>
       </c>
       <c r="C3062" t="inlineStr">
         <is>
-          <t>DGEO</t>
+          <t>DECA</t>
         </is>
       </c>
       <c r="D3062" t="inlineStr"/>
@@ -83282,18 +83282,18 @@
       <c r="F3062" t="inlineStr"/>
       <c r="G3062" t="inlineStr">
         <is>
-          <t xml:space="preserve">6542_Geologia de Campo - Ambientes Sedimentares </t>
+          <t>6539_Técnicas Contemporâneas de Composição e Arranjo em Jazz</t>
         </is>
       </c>
       <c r="H3062" t="inlineStr"/>
     </row>
     <row r="3063">
       <c r="A3063" t="n">
-        <v>65159</v>
+        <v>65158</v>
       </c>
       <c r="B3063" t="inlineStr">
         <is>
-          <t xml:space="preserve">GEOLOGIA DE CAMPO – ROCHAS METAMÓRFICAS </t>
+          <t xml:space="preserve">GEOLOGIA DE CAMPO - AMBIENTES SEDIMENTARES </t>
         </is>
       </c>
       <c r="C3063" t="inlineStr">
@@ -83306,18 +83306,18 @@
       <c r="F3063" t="inlineStr"/>
       <c r="G3063" t="inlineStr">
         <is>
-          <t xml:space="preserve">6543_Geologia de Campo – Rochas Metamórficas </t>
+          <t xml:space="preserve">6542_Geologia de Campo - Ambientes Sedimentares </t>
         </is>
       </c>
       <c r="H3063" t="inlineStr"/>
     </row>
     <row r="3064">
       <c r="A3064" t="n">
-        <v>65160</v>
+        <v>65159</v>
       </c>
       <c r="B3064" t="inlineStr">
         <is>
-          <t>GEOLOGIA DE CAMPO – ROCHAS ÍGNEAS</t>
+          <t xml:space="preserve">GEOLOGIA DE CAMPO – ROCHAS METAMÓRFICAS </t>
         </is>
       </c>
       <c r="C3064" t="inlineStr">
@@ -83330,10 +83330,34 @@
       <c r="F3064" t="inlineStr"/>
       <c r="G3064" t="inlineStr">
         <is>
+          <t xml:space="preserve">6543_Geologia de Campo – Rochas Metamórficas </t>
+        </is>
+      </c>
+      <c r="H3064" t="inlineStr"/>
+    </row>
+    <row r="3065">
+      <c r="A3065" t="n">
+        <v>65160</v>
+      </c>
+      <c r="B3065" t="inlineStr">
+        <is>
+          <t>GEOLOGIA DE CAMPO – ROCHAS ÍGNEAS</t>
+        </is>
+      </c>
+      <c r="C3065" t="inlineStr">
+        <is>
+          <t>DGEO</t>
+        </is>
+      </c>
+      <c r="D3065" t="inlineStr"/>
+      <c r="E3065" t="inlineStr"/>
+      <c r="F3065" t="inlineStr"/>
+      <c r="G3065" t="inlineStr">
+        <is>
           <t>6544_Geologia de Campo – Rochas Ígneas</t>
         </is>
       </c>
-      <c r="H3064" t="inlineStr"/>
+      <c r="H3065" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>